<commit_message>
Subjects Class and methods added with some changes in the main file
</commit_message>
<xml_diff>
--- a/student_management_system/data/subjects_data.xlsx
+++ b/student_management_system/data/subjects_data.xlsx
@@ -1,58 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
+  <bookViews>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+  </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -60,18 +45,94 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -150,7 +211,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -185,7 +245,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -220,16 +279,20 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="350000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -351,77 +414,82 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:spDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </a:style>
-    </a:spDef>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="str">
-        <v>subject_code</v>
-      </c>
-      <c r="B1" t="str">
-        <v>subject_name</v>
-      </c>
-      <c r="C1" t="str">
-        <v>subject_credit_theory</v>
-      </c>
-      <c r="D1" t="str">
-        <v>subject_credit_practical</v>
-      </c>
-      <c r="E1" t="str">
-        <v>taught_in_sem</v>
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>subject_code</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>subject_credit_practical</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>subject_credit_theory</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>subject_name</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>taught_in_branch</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>taught_in_sem</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>123</v>
+      </c>
+      <c r="B2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" t="n">
+        <v>3</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>ABC</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>CE,IT</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E1"/>
-  </ignoredErrors>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>